<commit_message>
Projeto corrigido de QA
</commit_message>
<xml_diff>
--- a/Sprint-1/Vinicius Fischer, 8º grupo — 1º sprint.xlsx
+++ b/Sprint-1/Vinicius Fischer, 8º grupo — 1º sprint.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="181">
   <si>
     <r>
       <rPr>
@@ -542,9 +542,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Arpovado </t>
-  </si>
-  <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
@@ -1428,28 +1425,28 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Os títulos das cidades no mapa são clicaveis e não deveria acontecer </t>
+    <t xml:space="preserve">Os títulos das cidades no mapa são clicáveis e não deveria acontecer </t>
   </si>
   <si>
     <t>Abra o aplicativo Urban Routes Clique no nome do local presente no mapa por exemplo: "Hollywood".</t>
   </si>
   <si>
-    <t>Aparece um balão com a localizção e um botão para redirecionar o usuario ao google maps</t>
+    <t>Aparece um balão com a localização e um botão para redirecionar o usuário ao google maps</t>
   </si>
   <si>
     <t xml:space="preserve">Pequeno </t>
   </si>
   <si>
-    <t>O campo "De" pode ser selecionado porem ele não esta vazio.</t>
+    <t>O campo "De" pode ser selecionado porém ele não está vazio.</t>
   </si>
   <si>
     <t>Abra o aplicativo Urban Routes clique no campo "De"</t>
   </si>
   <si>
-    <t>O campo de pesquisa não fica vazio, aparece uma exemplo em marca d'agua "East 2nd Street, 601"</t>
-  </si>
-  <si>
-    <t>Não é possivel pesquisar objetos no campo "Para"</t>
+    <t>O campo de pesquisa não fica vazio, aparece uma exemplo em marca d'água "East 2nd Street, 601"</t>
+  </si>
+  <si>
+    <t>Não é possível pesquisar objetos no campo "Para"</t>
   </si>
   <si>
     <t>Abra o aplicativo Urban Routes clique no campo "Para" digite "Subway".</t>
@@ -1461,10 +1458,10 @@
     <t>Grave</t>
   </si>
   <si>
-    <t xml:space="preserve">O pino de endereço não aparece apos prencher o campo "De" </t>
-  </si>
-  <si>
-    <t>Abra o aplicatico Urban Routes clique no campo "De" e escreva o endereço Ex: East 2nd Street, 601</t>
+    <t xml:space="preserve">O pino de endereço não aparece após preencher o campo "De" </t>
+  </si>
+  <si>
+    <t>Abra o aplicativo Urban Routes clique no campo "De" e escreva o endereço Ex: East 2nd Street, 601</t>
   </si>
   <si>
     <t xml:space="preserve">Nada acontece no mapa </t>
@@ -1473,10 +1470,10 @@
     <t xml:space="preserve">Grave </t>
   </si>
   <si>
-    <t>O pino de endereço não aparece apos prencher o campo "Para"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Abra o aplicatico Urban Routes clique no campo "Para" e escreva o endereço Ex: 1300 1st St </t>
+    <t>O pino de endereço não aparece após preencher o campo "Para"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abra o aplicativo Urban Routes clique no campo "Para" e escreva o endereço Ex: 1300 1st St </t>
   </si>
   <si>
     <t xml:space="preserve">As informações do aplicativo não são exibidas ao clicar no logotipo </t>
@@ -2206,132 +2203,132 @@
         <v>65</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" ht="70.5" customHeight="1">
       <c r="A15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="D15" s="2">
         <v>1.0</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" ht="63.0" customHeight="1">
       <c r="A16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="D16" s="2">
         <v>1.0</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" ht="124.5" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D17" s="2">
         <v>1.0</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="10"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D18" s="2">
         <v>1.0</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="10"/>
     </row>
     <row r="19" ht="48.0" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="D19" s="2">
         <v>1.0</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="G19" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="10"/>
@@ -2344,7 +2341,7 @@
         <v>2.0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
@@ -2359,7 +2356,7 @@
         <v>3.0</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -2368,22 +2365,22 @@
     </row>
     <row r="22" ht="48.75" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="D22" s="2">
         <v>1.0</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>13</v>
@@ -2399,7 +2396,7 @@
         <v>2.0</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -2408,22 +2405,22 @@
     </row>
     <row r="24" ht="68.25" customHeight="1">
       <c r="A24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="D24" s="2">
         <v>1.0</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>13</v>
@@ -2433,22 +2430,22 @@
     </row>
     <row r="25" ht="60.75" customHeight="1">
       <c r="A25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D25" s="2">
         <v>1.0</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>13</v>
@@ -2458,22 +2455,22 @@
     </row>
     <row r="26" ht="66.0" customHeight="1">
       <c r="A26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="D26" s="2">
         <v>1.0</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>13</v>
@@ -2483,22 +2480,22 @@
     </row>
     <row r="27" ht="76.5" customHeight="1">
       <c r="A27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="D27" s="2">
         <v>1.0</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>13</v>
@@ -2508,22 +2505,22 @@
     </row>
     <row r="28" ht="83.25" customHeight="1">
       <c r="A28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="D28" s="2">
         <v>1.0</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>13</v>
@@ -2533,22 +2530,22 @@
     </row>
     <row r="29" ht="83.25" customHeight="1">
       <c r="A29" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>128</v>
       </c>
       <c r="D29" s="2">
         <v>1.0</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>13</v>
@@ -2558,22 +2555,22 @@
     </row>
     <row r="30" ht="65.25" customHeight="1">
       <c r="A30" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="D30" s="2">
         <v>1.0</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>13</v>
@@ -2589,10 +2586,10 @@
         <v>2.0</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="G31" s="11"/>
       <c r="H31" s="11"/>
@@ -2606,10 +2603,10 @@
         <v>3.0</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
@@ -2623,10 +2620,10 @@
         <v>4.0</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
@@ -2640,10 +2637,10 @@
         <v>5.0</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
@@ -2651,53 +2648,53 @@
     </row>
     <row r="35" ht="93.75" customHeight="1">
       <c r="A35" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="D35" s="2">
         <v>1.0</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="G35" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="10"/>
     </row>
     <row r="36" ht="80.25" customHeight="1">
       <c r="A36" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="D36" s="2">
         <v>1.0</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I36" s="10"/>
     </row>
@@ -5538,22 +5535,22 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>160</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="15"/>
@@ -5581,19 +5578,19 @@
         <v>26</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>162</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="F2" s="16" t="s">
         <v>163</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>164</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -5621,19 +5618,19 @@
         <v>37</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>166</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -5661,19 +5658,19 @@
         <v>43</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>168</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>169</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>170</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>171</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -5701,19 +5698,19 @@
         <v>50</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>172</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>173</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>174</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>175</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -5741,19 +5738,19 @@
         <v>58</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>176</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>177</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
@@ -5778,22 +5775,22 @@
     </row>
     <row r="7" ht="50.25" customHeight="1">
       <c r="A7" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B7" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="D7" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>181</v>
-      </c>
       <c r="F7" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>

</xml_diff>